<commit_message>
Update graph and experiments
</commit_message>
<xml_diff>
--- a/results/summary_graph_classification_GCN_brf.csv.xlsx
+++ b/results/summary_graph_classification_GCN_brf.csv.xlsx
@@ -453,16 +453,16 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <v>27.83333333333333</v>
+        <v>32</v>
       </c>
       <c r="D3">
-        <v>0.0276686746259295</v>
+        <v>0.0315524255098646</v>
       </c>
       <c r="E3">
         <v>5</v>
       </c>
       <c r="F3">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:6">

</xml_diff>